<commit_message>
BA Evaluasi Pra kelar + Daftar hadir tapi belom $PP
</commit_message>
<xml_diff>
--- a/templates/Daftar Hadir Prakualifikasi.xlsx
+++ b/templates/Daftar Hadir Prakualifikasi.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="20115" windowHeight="8505"/>
+    <workbookView xWindow="240" yWindow="100" windowWidth="23240" windowHeight="14280"/>
   </bookViews>
   <sheets>
     <sheet name="Daftar Hadir" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -279,7 +284,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -332,149 +337,152 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3106,124 +3114,126 @@
   <dimension ref="A1:L85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="I4" sqref="I4:K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="1.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="1.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+    <row r="1" spans="1:11" ht="17">
+      <c r="A1" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-    </row>
-    <row r="2" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="75" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+    </row>
+    <row r="2" spans="1:11" ht="18" customHeight="1">
+      <c r="A2" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-    </row>
-    <row r="3" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+    </row>
+    <row r="3" spans="1:11" ht="18" customHeight="1">
       <c r="A3" s="23"/>
       <c r="B3" s="23"/>
       <c r="C3" t="s">
         <v>18</v>
       </c>
       <c r="D3" s="23"/>
-      <c r="E3" s="73" t="s">
+      <c r="E3" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="73"/>
+      <c r="F3" s="41"/>
       <c r="G3" s="23"/>
       <c r="H3" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="73" t="s">
+      <c r="I3" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="73"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J3" s="41"/>
+    </row>
+    <row r="4" spans="1:11" ht="17" customHeight="1">
       <c r="A4" s="24"/>
       <c r="B4" s="25"/>
       <c r="C4" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="25"/>
-      <c r="E4" s="74" t="s">
+      <c r="E4" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="74"/>
+      <c r="F4" s="42"/>
       <c r="G4" s="25"/>
       <c r="H4" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="74" t="s">
+      <c r="I4" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="74"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J4" s="76"/>
+      <c r="K4" s="76"/>
+    </row>
+    <row r="5" spans="1:11">
       <c r="J5" s="26"/>
       <c r="K5" s="26"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="61" t="s">
+    <row r="6" spans="1:11">
+      <c r="A6" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="62"/>
-      <c r="C6" s="65" t="s">
+      <c r="B6" s="30"/>
+      <c r="C6" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="66"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="61" t="s">
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="71"/>
-      <c r="I6" s="71"/>
-      <c r="J6" s="71"/>
-      <c r="K6" s="62"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="63"/>
-      <c r="B7" s="64"/>
-      <c r="C7" s="68"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="70"/>
-      <c r="G7" s="63"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="72"/>
-      <c r="J7" s="72"/>
-      <c r="K7" s="64"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="30"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="31"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="32"/>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -3234,41 +3244,41 @@
       <c r="D8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="41"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="31"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E8" s="71"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="46"/>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="C9" s="15"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="31"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E9" s="71"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="45"/>
+      <c r="K9" s="46"/>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="17"/>
       <c r="D10" s="6"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="31"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E10" s="72"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="45"/>
+      <c r="K10" s="46"/>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="18" t="s">
@@ -3277,41 +3287,41 @@
       <c r="D11" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="31"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E11" s="75"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="45"/>
+      <c r="K11" s="46"/>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="C12" s="15"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="31"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E12" s="71"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="45"/>
+      <c r="K12" s="46"/>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="17"/>
       <c r="D13" s="6"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="31"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E13" s="72"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="45"/>
+      <c r="J13" s="45"/>
+      <c r="K13" s="46"/>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="C14" s="15" t="s">
@@ -3320,15 +3330,15 @@
       <c r="D14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="59"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35"/>
-      <c r="K14" s="31"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E14" s="53"/>
+      <c r="F14" s="54"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="45"/>
+      <c r="J14" s="45"/>
+      <c r="K14" s="46"/>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="C15" s="19" t="s">
@@ -3337,15 +3347,15 @@
       <c r="D15" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E15" s="58"/>
-      <c r="F15" s="46"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="35"/>
-      <c r="K15" s="31"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E15" s="55"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="45"/>
+      <c r="J15" s="45"/>
+      <c r="K15" s="46"/>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="15" t="s">
@@ -3354,15 +3364,15 @@
       <c r="D16" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="56"/>
-      <c r="F16" s="57"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
-      <c r="K16" s="31"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E16" s="73"/>
+      <c r="F16" s="74"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="45"/>
+      <c r="J16" s="45"/>
+      <c r="K16" s="46"/>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="21" t="s">
@@ -3371,15 +3381,15 @@
       <c r="D17" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E17" s="58"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
-      <c r="K17" s="31"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E17" s="55"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="45"/>
+      <c r="J17" s="45"/>
+      <c r="K17" s="46"/>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="C18" s="15" t="s">
@@ -3388,15 +3398,15 @@
       <c r="D18" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E18" s="35"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="31"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E18" s="45"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="45"/>
+      <c r="K18" s="46"/>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" s="1"/>
       <c r="B19" s="3"/>
       <c r="C19" s="16" t="s">
@@ -3405,28 +3415,28 @@
       <c r="D19" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="32"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="35"/>
-      <c r="K19" s="31"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E19" s="61"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="45"/>
+      <c r="J19" s="45"/>
+      <c r="K19" s="46"/>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" s="5"/>
       <c r="B20" s="7"/>
       <c r="C20" s="17"/>
       <c r="D20" s="7"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="37"/>
-      <c r="J20" s="37"/>
-      <c r="K20" s="38"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E20" s="62"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="47"/>
+      <c r="I20" s="47"/>
+      <c r="J20" s="47"/>
+      <c r="K20" s="48"/>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" s="1">
         <v>2</v>
       </c>
@@ -3437,41 +3447,41 @@
       <c r="D21" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E21" s="51"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="33"/>
-      <c r="K21" s="34"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E21" s="63"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="49"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="49"/>
+      <c r="K21" s="50"/>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="C22" s="15"/>
       <c r="D22" s="3"/>
-      <c r="E22" s="52"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="35"/>
-      <c r="I22" s="35"/>
-      <c r="J22" s="35"/>
-      <c r="K22" s="31"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E22" s="65"/>
+      <c r="F22" s="66"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="45"/>
+      <c r="I22" s="45"/>
+      <c r="J22" s="45"/>
+      <c r="K22" s="46"/>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="C23" s="17"/>
       <c r="D23" s="7"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="35"/>
-      <c r="I23" s="35"/>
-      <c r="J23" s="35"/>
-      <c r="K23" s="31"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E23" s="67"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="45"/>
+      <c r="K23" s="46"/>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="C24" s="18" t="s">
@@ -3480,41 +3490,41 @@
       <c r="D24" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E24" s="52"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="30"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="35"/>
-      <c r="J24" s="35"/>
-      <c r="K24" s="31"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E24" s="65"/>
+      <c r="F24" s="66"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="45"/>
+      <c r="I24" s="45"/>
+      <c r="J24" s="45"/>
+      <c r="K24" s="46"/>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="C25" s="15"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="52"/>
-      <c r="F25" s="42"/>
-      <c r="G25" s="30"/>
-      <c r="H25" s="35"/>
-      <c r="I25" s="35"/>
-      <c r="J25" s="35"/>
-      <c r="K25" s="31"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E25" s="65"/>
+      <c r="F25" s="66"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="45"/>
+      <c r="I25" s="45"/>
+      <c r="J25" s="45"/>
+      <c r="K25" s="46"/>
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="C26" s="17"/>
       <c r="D26" s="3"/>
-      <c r="E26" s="52"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="35"/>
-      <c r="I26" s="35"/>
-      <c r="J26" s="35"/>
-      <c r="K26" s="31"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E26" s="65"/>
+      <c r="F26" s="66"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="45"/>
+      <c r="I26" s="45"/>
+      <c r="J26" s="45"/>
+      <c r="K26" s="46"/>
+    </row>
+    <row r="27" spans="1:11">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="C27" s="15" t="s">
@@ -3523,15 +3533,15 @@
       <c r="D27" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E27" s="45"/>
-      <c r="F27" s="46"/>
-      <c r="G27" s="35"/>
-      <c r="H27" s="35"/>
-      <c r="I27" s="35"/>
-      <c r="J27" s="35"/>
-      <c r="K27" s="31"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E27" s="51"/>
+      <c r="F27" s="52"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="45"/>
+      <c r="I27" s="45"/>
+      <c r="J27" s="45"/>
+      <c r="K27" s="46"/>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="C28" s="19" t="s">
@@ -3540,15 +3550,15 @@
       <c r="D28" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E28" s="47"/>
-      <c r="F28" s="48"/>
-      <c r="G28" s="30"/>
-      <c r="H28" s="35"/>
-      <c r="I28" s="35"/>
-      <c r="J28" s="35"/>
-      <c r="K28" s="31"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E28" s="56"/>
+      <c r="F28" s="54"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="45"/>
+      <c r="K28" s="46"/>
+    </row>
+    <row r="29" spans="1:11">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="C29" s="15" t="s">
@@ -3557,15 +3567,15 @@
       <c r="D29" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E29" s="49"/>
-      <c r="F29" s="50"/>
-      <c r="G29" s="35"/>
-      <c r="H29" s="35"/>
-      <c r="I29" s="35"/>
-      <c r="J29" s="35"/>
-      <c r="K29" s="31"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E29" s="57"/>
+      <c r="F29" s="58"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
+      <c r="K29" s="46"/>
+    </row>
+    <row r="30" spans="1:11">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="C30" s="21" t="s">
@@ -3574,15 +3584,15 @@
       <c r="D30" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E30" s="47"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="35"/>
-      <c r="I30" s="35"/>
-      <c r="J30" s="35"/>
-      <c r="K30" s="31"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E30" s="56"/>
+      <c r="F30" s="54"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
+      <c r="K30" s="46"/>
+    </row>
+    <row r="31" spans="1:11">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="C31" s="15" t="s">
@@ -3591,15 +3601,15 @@
       <c r="D31" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E31" s="28"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="35"/>
-      <c r="H31" s="35"/>
-      <c r="I31" s="35"/>
-      <c r="J31" s="35"/>
-      <c r="K31" s="31"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E31" s="59"/>
+      <c r="F31" s="60"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="45"/>
+      <c r="I31" s="45"/>
+      <c r="J31" s="45"/>
+      <c r="K31" s="46"/>
+    </row>
+    <row r="32" spans="1:11">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="C32" s="16" t="s">
@@ -3608,28 +3618,28 @@
       <c r="D32" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E32" s="30"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="30"/>
-      <c r="H32" s="35"/>
-      <c r="I32" s="35"/>
-      <c r="J32" s="35"/>
-      <c r="K32" s="31"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E32" s="44"/>
+      <c r="F32" s="46"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="45"/>
+      <c r="I32" s="45"/>
+      <c r="J32" s="45"/>
+      <c r="K32" s="46"/>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="C33" s="13"/>
       <c r="D33" s="3"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="35"/>
-      <c r="I33" s="35"/>
-      <c r="J33" s="35"/>
-      <c r="K33" s="31"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E33" s="44"/>
+      <c r="F33" s="46"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="45"/>
+      <c r="I33" s="45"/>
+      <c r="J33" s="45"/>
+      <c r="K33" s="46"/>
+    </row>
+    <row r="34" spans="1:12">
       <c r="A34" s="8">
         <v>3</v>
       </c>
@@ -3640,44 +3650,44 @@
       <c r="D34" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="E34" s="51"/>
-      <c r="F34" s="40"/>
-      <c r="G34" s="32"/>
-      <c r="H34" s="33"/>
-      <c r="I34" s="33"/>
-      <c r="J34" s="33"/>
-      <c r="K34" s="34"/>
+      <c r="E34" s="63"/>
+      <c r="F34" s="64"/>
+      <c r="G34" s="61"/>
+      <c r="H34" s="49"/>
+      <c r="I34" s="49"/>
+      <c r="J34" s="49"/>
+      <c r="K34" s="50"/>
       <c r="L34" s="3"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="C35" s="15"/>
       <c r="D35" s="2"/>
-      <c r="E35" s="52"/>
-      <c r="F35" s="42"/>
-      <c r="G35" s="30"/>
-      <c r="H35" s="35"/>
-      <c r="I35" s="35"/>
-      <c r="J35" s="35"/>
-      <c r="K35" s="31"/>
+      <c r="E35" s="65"/>
+      <c r="F35" s="66"/>
+      <c r="G35" s="44"/>
+      <c r="H35" s="45"/>
+      <c r="I35" s="45"/>
+      <c r="J35" s="45"/>
+      <c r="K35" s="46"/>
       <c r="L35" s="3"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="C36" s="17"/>
       <c r="D36" s="6"/>
-      <c r="E36" s="53"/>
-      <c r="F36" s="44"/>
-      <c r="G36" s="30"/>
-      <c r="H36" s="35"/>
-      <c r="I36" s="35"/>
-      <c r="J36" s="35"/>
-      <c r="K36" s="31"/>
+      <c r="E36" s="67"/>
+      <c r="F36" s="68"/>
+      <c r="G36" s="44"/>
+      <c r="H36" s="45"/>
+      <c r="I36" s="45"/>
+      <c r="J36" s="45"/>
+      <c r="K36" s="46"/>
       <c r="L36" s="3"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="C37" s="18" t="s">
@@ -3686,44 +3696,44 @@
       <c r="D37" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E37" s="52"/>
-      <c r="F37" s="42"/>
-      <c r="G37" s="30"/>
-      <c r="H37" s="35"/>
-      <c r="I37" s="35"/>
-      <c r="J37" s="35"/>
-      <c r="K37" s="31"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="66"/>
+      <c r="G37" s="44"/>
+      <c r="H37" s="45"/>
+      <c r="I37" s="45"/>
+      <c r="J37" s="45"/>
+      <c r="K37" s="46"/>
       <c r="L37" s="3"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="C38" s="15"/>
       <c r="D38" s="3"/>
-      <c r="E38" s="52"/>
-      <c r="F38" s="42"/>
-      <c r="G38" s="30"/>
-      <c r="H38" s="35"/>
-      <c r="I38" s="35"/>
-      <c r="J38" s="35"/>
-      <c r="K38" s="31"/>
+      <c r="E38" s="65"/>
+      <c r="F38" s="66"/>
+      <c r="G38" s="44"/>
+      <c r="H38" s="45"/>
+      <c r="I38" s="45"/>
+      <c r="J38" s="45"/>
+      <c r="K38" s="46"/>
       <c r="L38" s="3"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="C39" s="17"/>
       <c r="D39" s="3"/>
-      <c r="E39" s="52"/>
-      <c r="F39" s="42"/>
-      <c r="G39" s="30"/>
-      <c r="H39" s="35"/>
-      <c r="I39" s="35"/>
-      <c r="J39" s="35"/>
-      <c r="K39" s="31"/>
+      <c r="E39" s="65"/>
+      <c r="F39" s="66"/>
+      <c r="G39" s="44"/>
+      <c r="H39" s="45"/>
+      <c r="I39" s="45"/>
+      <c r="J39" s="45"/>
+      <c r="K39" s="46"/>
       <c r="L39" s="3"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="C40" s="15" t="s">
@@ -3732,16 +3742,16 @@
       <c r="D40" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E40" s="45"/>
-      <c r="F40" s="46"/>
-      <c r="G40" s="30"/>
-      <c r="H40" s="35"/>
-      <c r="I40" s="35"/>
-      <c r="J40" s="35"/>
-      <c r="K40" s="31"/>
+      <c r="E40" s="51"/>
+      <c r="F40" s="52"/>
+      <c r="G40" s="44"/>
+      <c r="H40" s="45"/>
+      <c r="I40" s="45"/>
+      <c r="J40" s="45"/>
+      <c r="K40" s="46"/>
       <c r="L40" s="3"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="C41" s="19" t="s">
@@ -3750,16 +3760,16 @@
       <c r="D41" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E41" s="47"/>
-      <c r="F41" s="48"/>
-      <c r="G41" s="30"/>
-      <c r="H41" s="35"/>
-      <c r="I41" s="35"/>
-      <c r="J41" s="35"/>
-      <c r="K41" s="31"/>
+      <c r="E41" s="56"/>
+      <c r="F41" s="54"/>
+      <c r="G41" s="44"/>
+      <c r="H41" s="45"/>
+      <c r="I41" s="45"/>
+      <c r="J41" s="45"/>
+      <c r="K41" s="46"/>
       <c r="L41" s="3"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="C42" s="15" t="s">
@@ -3768,16 +3778,16 @@
       <c r="D42" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E42" s="49"/>
-      <c r="F42" s="50"/>
-      <c r="G42" s="30"/>
-      <c r="H42" s="35"/>
-      <c r="I42" s="35"/>
-      <c r="J42" s="35"/>
-      <c r="K42" s="31"/>
+      <c r="E42" s="57"/>
+      <c r="F42" s="58"/>
+      <c r="G42" s="44"/>
+      <c r="H42" s="45"/>
+      <c r="I42" s="45"/>
+      <c r="J42" s="45"/>
+      <c r="K42" s="46"/>
       <c r="L42" s="3"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="C43" s="21" t="s">
@@ -3786,16 +3796,16 @@
       <c r="D43" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E43" s="47"/>
-      <c r="F43" s="48"/>
-      <c r="G43" s="30"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
-      <c r="K43" s="31"/>
+      <c r="E43" s="56"/>
+      <c r="F43" s="54"/>
+      <c r="G43" s="44"/>
+      <c r="H43" s="45"/>
+      <c r="I43" s="45"/>
+      <c r="J43" s="45"/>
+      <c r="K43" s="46"/>
       <c r="L43" s="3"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="C44" s="15" t="s">
@@ -3804,16 +3814,16 @@
       <c r="D44" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E44" s="28"/>
-      <c r="F44" s="29"/>
-      <c r="G44" s="30"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
-      <c r="K44" s="31"/>
+      <c r="E44" s="59"/>
+      <c r="F44" s="60"/>
+      <c r="G44" s="44"/>
+      <c r="H44" s="45"/>
+      <c r="I44" s="45"/>
+      <c r="J44" s="45"/>
+      <c r="K44" s="46"/>
       <c r="L44" s="3"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="C45" s="16" t="s">
@@ -3822,30 +3832,30 @@
       <c r="D45" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E45" s="30"/>
-      <c r="F45" s="31"/>
-      <c r="G45" s="30"/>
-      <c r="H45" s="35"/>
-      <c r="I45" s="35"/>
-      <c r="J45" s="35"/>
-      <c r="K45" s="31"/>
+      <c r="E45" s="44"/>
+      <c r="F45" s="46"/>
+      <c r="G45" s="44"/>
+      <c r="H45" s="45"/>
+      <c r="I45" s="45"/>
+      <c r="J45" s="45"/>
+      <c r="K45" s="46"/>
       <c r="L45" s="3"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12">
       <c r="A46" s="5"/>
       <c r="B46" s="6"/>
       <c r="C46" s="17"/>
       <c r="D46" s="7"/>
-      <c r="E46" s="36"/>
-      <c r="F46" s="38"/>
-      <c r="G46" s="36"/>
-      <c r="H46" s="37"/>
-      <c r="I46" s="37"/>
-      <c r="J46" s="37"/>
-      <c r="K46" s="38"/>
+      <c r="E46" s="62"/>
+      <c r="F46" s="48"/>
+      <c r="G46" s="62"/>
+      <c r="H46" s="47"/>
+      <c r="I46" s="47"/>
+      <c r="J46" s="47"/>
+      <c r="K46" s="48"/>
       <c r="L46" s="3"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12">
       <c r="A47" s="8">
         <v>4</v>
       </c>
@@ -3856,44 +3866,44 @@
       <c r="D47" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E47" s="51"/>
-      <c r="F47" s="40"/>
-      <c r="G47" s="32"/>
-      <c r="H47" s="33"/>
-      <c r="I47" s="33"/>
-      <c r="J47" s="33"/>
-      <c r="K47" s="34"/>
+      <c r="E47" s="63"/>
+      <c r="F47" s="64"/>
+      <c r="G47" s="61"/>
+      <c r="H47" s="49"/>
+      <c r="I47" s="49"/>
+      <c r="J47" s="49"/>
+      <c r="K47" s="50"/>
       <c r="L47" s="3"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="C48" s="15"/>
       <c r="D48" s="3"/>
-      <c r="E48" s="52"/>
-      <c r="F48" s="42"/>
-      <c r="G48" s="30"/>
-      <c r="H48" s="35"/>
-      <c r="I48" s="35"/>
-      <c r="J48" s="35"/>
-      <c r="K48" s="31"/>
+      <c r="E48" s="65"/>
+      <c r="F48" s="66"/>
+      <c r="G48" s="44"/>
+      <c r="H48" s="45"/>
+      <c r="I48" s="45"/>
+      <c r="J48" s="45"/>
+      <c r="K48" s="46"/>
       <c r="L48" s="3"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="C49" s="17"/>
       <c r="D49" s="7"/>
-      <c r="E49" s="53"/>
-      <c r="F49" s="44"/>
-      <c r="G49" s="30"/>
-      <c r="H49" s="35"/>
-      <c r="I49" s="35"/>
-      <c r="J49" s="35"/>
-      <c r="K49" s="31"/>
+      <c r="E49" s="67"/>
+      <c r="F49" s="68"/>
+      <c r="G49" s="44"/>
+      <c r="H49" s="45"/>
+      <c r="I49" s="45"/>
+      <c r="J49" s="45"/>
+      <c r="K49" s="46"/>
       <c r="L49" s="3"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="C50" s="18" t="s">
@@ -3902,44 +3912,44 @@
       <c r="D50" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E50" s="54"/>
-      <c r="F50" s="55"/>
-      <c r="G50" s="30"/>
-      <c r="H50" s="35"/>
-      <c r="I50" s="35"/>
-      <c r="J50" s="35"/>
-      <c r="K50" s="31"/>
+      <c r="E50" s="69"/>
+      <c r="F50" s="70"/>
+      <c r="G50" s="44"/>
+      <c r="H50" s="45"/>
+      <c r="I50" s="45"/>
+      <c r="J50" s="45"/>
+      <c r="K50" s="46"/>
       <c r="L50" s="3"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
       <c r="C51" s="15"/>
       <c r="D51" s="3"/>
-      <c r="E51" s="54"/>
-      <c r="F51" s="55"/>
-      <c r="G51" s="30"/>
-      <c r="H51" s="35"/>
-      <c r="I51" s="35"/>
-      <c r="J51" s="35"/>
-      <c r="K51" s="31"/>
+      <c r="E51" s="69"/>
+      <c r="F51" s="70"/>
+      <c r="G51" s="44"/>
+      <c r="H51" s="45"/>
+      <c r="I51" s="45"/>
+      <c r="J51" s="45"/>
+      <c r="K51" s="46"/>
       <c r="L51" s="3"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="C52" s="17"/>
       <c r="D52" s="3"/>
-      <c r="E52" s="54"/>
-      <c r="F52" s="55"/>
-      <c r="G52" s="30"/>
-      <c r="H52" s="35"/>
-      <c r="I52" s="35"/>
-      <c r="J52" s="35"/>
-      <c r="K52" s="31"/>
+      <c r="E52" s="69"/>
+      <c r="F52" s="70"/>
+      <c r="G52" s="44"/>
+      <c r="H52" s="45"/>
+      <c r="I52" s="45"/>
+      <c r="J52" s="45"/>
+      <c r="K52" s="46"/>
       <c r="L52" s="3"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="C53" s="15" t="s">
@@ -3948,16 +3958,16 @@
       <c r="D53" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E53" s="45"/>
-      <c r="F53" s="46"/>
-      <c r="G53" s="30"/>
-      <c r="H53" s="35"/>
-      <c r="I53" s="35"/>
-      <c r="J53" s="35"/>
-      <c r="K53" s="31"/>
+      <c r="E53" s="51"/>
+      <c r="F53" s="52"/>
+      <c r="G53" s="44"/>
+      <c r="H53" s="45"/>
+      <c r="I53" s="45"/>
+      <c r="J53" s="45"/>
+      <c r="K53" s="46"/>
       <c r="L53" s="3"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="C54" s="19" t="s">
@@ -3966,16 +3976,16 @@
       <c r="D54" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E54" s="47"/>
-      <c r="F54" s="48"/>
-      <c r="G54" s="30"/>
-      <c r="H54" s="35"/>
-      <c r="I54" s="35"/>
-      <c r="J54" s="35"/>
-      <c r="K54" s="31"/>
+      <c r="E54" s="56"/>
+      <c r="F54" s="54"/>
+      <c r="G54" s="44"/>
+      <c r="H54" s="45"/>
+      <c r="I54" s="45"/>
+      <c r="J54" s="45"/>
+      <c r="K54" s="46"/>
       <c r="L54" s="3"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="C55" s="15" t="s">
@@ -3984,16 +3994,16 @@
       <c r="D55" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E55" s="49"/>
-      <c r="F55" s="50"/>
-      <c r="G55" s="30"/>
-      <c r="H55" s="35"/>
-      <c r="I55" s="35"/>
-      <c r="J55" s="35"/>
-      <c r="K55" s="31"/>
+      <c r="E55" s="57"/>
+      <c r="F55" s="58"/>
+      <c r="G55" s="44"/>
+      <c r="H55" s="45"/>
+      <c r="I55" s="45"/>
+      <c r="J55" s="45"/>
+      <c r="K55" s="46"/>
       <c r="L55" s="3"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="C56" s="21" t="s">
@@ -4002,16 +4012,16 @@
       <c r="D56" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E56" s="47"/>
-      <c r="F56" s="48"/>
-      <c r="G56" s="30"/>
-      <c r="H56" s="35"/>
-      <c r="I56" s="35"/>
-      <c r="J56" s="35"/>
-      <c r="K56" s="31"/>
+      <c r="E56" s="56"/>
+      <c r="F56" s="54"/>
+      <c r="G56" s="44"/>
+      <c r="H56" s="45"/>
+      <c r="I56" s="45"/>
+      <c r="J56" s="45"/>
+      <c r="K56" s="46"/>
       <c r="L56" s="3"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="C57" s="15" t="s">
@@ -4020,16 +4030,16 @@
       <c r="D57" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E57" s="28"/>
-      <c r="F57" s="29"/>
-      <c r="G57" s="30"/>
-      <c r="H57" s="35"/>
-      <c r="I57" s="35"/>
-      <c r="J57" s="35"/>
-      <c r="K57" s="31"/>
+      <c r="E57" s="59"/>
+      <c r="F57" s="60"/>
+      <c r="G57" s="44"/>
+      <c r="H57" s="45"/>
+      <c r="I57" s="45"/>
+      <c r="J57" s="45"/>
+      <c r="K57" s="46"/>
       <c r="L57" s="3"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="C58" s="16" t="s">
@@ -4038,30 +4048,30 @@
       <c r="D58" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E58" s="30"/>
-      <c r="F58" s="31"/>
-      <c r="G58" s="30"/>
-      <c r="H58" s="35"/>
-      <c r="I58" s="35"/>
-      <c r="J58" s="35"/>
-      <c r="K58" s="31"/>
+      <c r="E58" s="44"/>
+      <c r="F58" s="46"/>
+      <c r="G58" s="44"/>
+      <c r="H58" s="45"/>
+      <c r="I58" s="45"/>
+      <c r="J58" s="45"/>
+      <c r="K58" s="46"/>
       <c r="L58" s="3"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12">
       <c r="A59" s="5"/>
       <c r="B59" s="6"/>
       <c r="C59" s="14"/>
       <c r="D59" s="7"/>
-      <c r="E59" s="36"/>
-      <c r="F59" s="38"/>
-      <c r="G59" s="36"/>
-      <c r="H59" s="37"/>
-      <c r="I59" s="37"/>
-      <c r="J59" s="37"/>
-      <c r="K59" s="38"/>
+      <c r="E59" s="62"/>
+      <c r="F59" s="48"/>
+      <c r="G59" s="62"/>
+      <c r="H59" s="47"/>
+      <c r="I59" s="47"/>
+      <c r="J59" s="47"/>
+      <c r="K59" s="48"/>
       <c r="L59" s="3"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12">
       <c r="A60" s="8">
         <v>5</v>
       </c>
@@ -4072,44 +4082,44 @@
       <c r="D60" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E60" s="51"/>
-      <c r="F60" s="40"/>
-      <c r="G60" s="32"/>
-      <c r="H60" s="33"/>
-      <c r="I60" s="33"/>
-      <c r="J60" s="33"/>
-      <c r="K60" s="34"/>
+      <c r="E60" s="63"/>
+      <c r="F60" s="64"/>
+      <c r="G60" s="61"/>
+      <c r="H60" s="49"/>
+      <c r="I60" s="49"/>
+      <c r="J60" s="49"/>
+      <c r="K60" s="50"/>
       <c r="L60" s="3"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12">
       <c r="A61" s="1"/>
       <c r="B61" s="3"/>
       <c r="C61" s="15"/>
       <c r="D61" s="3"/>
-      <c r="E61" s="52"/>
-      <c r="F61" s="42"/>
-      <c r="G61" s="30"/>
-      <c r="H61" s="35"/>
-      <c r="I61" s="35"/>
-      <c r="J61" s="35"/>
-      <c r="K61" s="31"/>
+      <c r="E61" s="65"/>
+      <c r="F61" s="66"/>
+      <c r="G61" s="44"/>
+      <c r="H61" s="45"/>
+      <c r="I61" s="45"/>
+      <c r="J61" s="45"/>
+      <c r="K61" s="46"/>
       <c r="L61" s="3"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12">
       <c r="A62" s="1"/>
       <c r="B62" s="3"/>
       <c r="C62" s="17"/>
       <c r="D62" s="7"/>
-      <c r="E62" s="53"/>
-      <c r="F62" s="44"/>
-      <c r="G62" s="30"/>
-      <c r="H62" s="35"/>
-      <c r="I62" s="35"/>
-      <c r="J62" s="35"/>
-      <c r="K62" s="31"/>
+      <c r="E62" s="67"/>
+      <c r="F62" s="68"/>
+      <c r="G62" s="44"/>
+      <c r="H62" s="45"/>
+      <c r="I62" s="45"/>
+      <c r="J62" s="45"/>
+      <c r="K62" s="46"/>
       <c r="L62" s="3"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12">
       <c r="A63" s="1"/>
       <c r="B63" s="3"/>
       <c r="C63" s="18" t="s">
@@ -4118,44 +4128,44 @@
       <c r="D63" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E63" s="54"/>
-      <c r="F63" s="55"/>
-      <c r="G63" s="30"/>
-      <c r="H63" s="35"/>
-      <c r="I63" s="35"/>
-      <c r="J63" s="35"/>
-      <c r="K63" s="31"/>
+      <c r="E63" s="69"/>
+      <c r="F63" s="70"/>
+      <c r="G63" s="44"/>
+      <c r="H63" s="45"/>
+      <c r="I63" s="45"/>
+      <c r="J63" s="45"/>
+      <c r="K63" s="46"/>
       <c r="L63" s="3"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12">
       <c r="A64" s="1"/>
       <c r="B64" s="3"/>
       <c r="C64" s="15"/>
       <c r="D64" s="3"/>
-      <c r="E64" s="54"/>
-      <c r="F64" s="55"/>
-      <c r="G64" s="30"/>
-      <c r="H64" s="35"/>
-      <c r="I64" s="35"/>
-      <c r="J64" s="35"/>
-      <c r="K64" s="31"/>
+      <c r="E64" s="69"/>
+      <c r="F64" s="70"/>
+      <c r="G64" s="44"/>
+      <c r="H64" s="45"/>
+      <c r="I64" s="45"/>
+      <c r="J64" s="45"/>
+      <c r="K64" s="46"/>
       <c r="L64" s="3"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12">
       <c r="A65" s="1"/>
       <c r="B65" s="3"/>
       <c r="C65" s="17"/>
       <c r="D65" s="3"/>
-      <c r="E65" s="54"/>
-      <c r="F65" s="55"/>
-      <c r="G65" s="30"/>
-      <c r="H65" s="35"/>
-      <c r="I65" s="35"/>
-      <c r="J65" s="35"/>
-      <c r="K65" s="31"/>
+      <c r="E65" s="69"/>
+      <c r="F65" s="70"/>
+      <c r="G65" s="44"/>
+      <c r="H65" s="45"/>
+      <c r="I65" s="45"/>
+      <c r="J65" s="45"/>
+      <c r="K65" s="46"/>
       <c r="L65" s="3"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12">
       <c r="A66" s="1"/>
       <c r="B66" s="3"/>
       <c r="C66" s="15" t="s">
@@ -4164,16 +4174,16 @@
       <c r="D66" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E66" s="45"/>
-      <c r="F66" s="46"/>
-      <c r="G66" s="30"/>
-      <c r="H66" s="35"/>
-      <c r="I66" s="35"/>
-      <c r="J66" s="35"/>
-      <c r="K66" s="31"/>
+      <c r="E66" s="51"/>
+      <c r="F66" s="52"/>
+      <c r="G66" s="44"/>
+      <c r="H66" s="45"/>
+      <c r="I66" s="45"/>
+      <c r="J66" s="45"/>
+      <c r="K66" s="46"/>
       <c r="L66" s="3"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12">
       <c r="A67" s="1"/>
       <c r="B67" s="3"/>
       <c r="C67" s="19" t="s">
@@ -4182,16 +4192,16 @@
       <c r="D67" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E67" s="47"/>
-      <c r="F67" s="48"/>
-      <c r="G67" s="30"/>
-      <c r="H67" s="35"/>
-      <c r="I67" s="35"/>
-      <c r="J67" s="35"/>
-      <c r="K67" s="31"/>
+      <c r="E67" s="56"/>
+      <c r="F67" s="54"/>
+      <c r="G67" s="44"/>
+      <c r="H67" s="45"/>
+      <c r="I67" s="45"/>
+      <c r="J67" s="45"/>
+      <c r="K67" s="46"/>
       <c r="L67" s="3"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12">
       <c r="A68" s="1"/>
       <c r="B68" s="3"/>
       <c r="C68" s="15" t="s">
@@ -4200,16 +4210,16 @@
       <c r="D68" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E68" s="49"/>
-      <c r="F68" s="50"/>
-      <c r="G68" s="30"/>
-      <c r="H68" s="35"/>
-      <c r="I68" s="35"/>
-      <c r="J68" s="35"/>
-      <c r="K68" s="31"/>
+      <c r="E68" s="57"/>
+      <c r="F68" s="58"/>
+      <c r="G68" s="44"/>
+      <c r="H68" s="45"/>
+      <c r="I68" s="45"/>
+      <c r="J68" s="45"/>
+      <c r="K68" s="46"/>
       <c r="L68" s="3"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12">
       <c r="A69" s="1"/>
       <c r="B69" s="3"/>
       <c r="C69" s="21" t="s">
@@ -4218,16 +4228,16 @@
       <c r="D69" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E69" s="47"/>
-      <c r="F69" s="48"/>
-      <c r="G69" s="30"/>
-      <c r="H69" s="35"/>
-      <c r="I69" s="35"/>
-      <c r="J69" s="35"/>
-      <c r="K69" s="31"/>
+      <c r="E69" s="56"/>
+      <c r="F69" s="54"/>
+      <c r="G69" s="44"/>
+      <c r="H69" s="45"/>
+      <c r="I69" s="45"/>
+      <c r="J69" s="45"/>
+      <c r="K69" s="46"/>
       <c r="L69" s="3"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12">
       <c r="A70" s="1"/>
       <c r="B70" s="3"/>
       <c r="C70" s="15" t="s">
@@ -4236,16 +4246,16 @@
       <c r="D70" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E70" s="28"/>
-      <c r="F70" s="29"/>
-      <c r="G70" s="30"/>
-      <c r="H70" s="35"/>
-      <c r="I70" s="35"/>
-      <c r="J70" s="35"/>
-      <c r="K70" s="31"/>
+      <c r="E70" s="59"/>
+      <c r="F70" s="60"/>
+      <c r="G70" s="44"/>
+      <c r="H70" s="45"/>
+      <c r="I70" s="45"/>
+      <c r="J70" s="45"/>
+      <c r="K70" s="46"/>
       <c r="L70" s="3"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12">
       <c r="A71" s="1"/>
       <c r="B71" s="3"/>
       <c r="C71" s="16" t="s">
@@ -4254,30 +4264,30 @@
       <c r="D71" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E71" s="30"/>
-      <c r="F71" s="31"/>
-      <c r="G71" s="30"/>
-      <c r="H71" s="35"/>
-      <c r="I71" s="35"/>
-      <c r="J71" s="35"/>
-      <c r="K71" s="31"/>
+      <c r="E71" s="44"/>
+      <c r="F71" s="46"/>
+      <c r="G71" s="44"/>
+      <c r="H71" s="45"/>
+      <c r="I71" s="45"/>
+      <c r="J71" s="45"/>
+      <c r="K71" s="46"/>
       <c r="L71" s="3"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12">
       <c r="A72" s="1"/>
       <c r="B72" s="3"/>
       <c r="C72" s="15"/>
       <c r="D72" s="3"/>
-      <c r="E72" s="30"/>
-      <c r="F72" s="31"/>
-      <c r="G72" s="30"/>
-      <c r="H72" s="35"/>
-      <c r="I72" s="35"/>
-      <c r="J72" s="35"/>
-      <c r="K72" s="31"/>
+      <c r="E72" s="44"/>
+      <c r="F72" s="46"/>
+      <c r="G72" s="44"/>
+      <c r="H72" s="45"/>
+      <c r="I72" s="45"/>
+      <c r="J72" s="45"/>
+      <c r="K72" s="46"/>
       <c r="L72" s="3"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12">
       <c r="A73" s="8">
         <v>6</v>
       </c>
@@ -4288,44 +4298,44 @@
       <c r="D73" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="E73" s="51"/>
-      <c r="F73" s="40"/>
-      <c r="G73" s="32"/>
-      <c r="H73" s="33"/>
-      <c r="I73" s="33"/>
-      <c r="J73" s="33"/>
-      <c r="K73" s="34"/>
+      <c r="E73" s="63"/>
+      <c r="F73" s="64"/>
+      <c r="G73" s="61"/>
+      <c r="H73" s="49"/>
+      <c r="I73" s="49"/>
+      <c r="J73" s="49"/>
+      <c r="K73" s="50"/>
       <c r="L73" s="3"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12">
       <c r="A74" s="1"/>
       <c r="B74" s="3"/>
       <c r="C74" s="15"/>
       <c r="D74" s="2"/>
-      <c r="E74" s="52"/>
-      <c r="F74" s="42"/>
-      <c r="G74" s="30"/>
-      <c r="H74" s="35"/>
-      <c r="I74" s="35"/>
-      <c r="J74" s="35"/>
-      <c r="K74" s="31"/>
+      <c r="E74" s="65"/>
+      <c r="F74" s="66"/>
+      <c r="G74" s="44"/>
+      <c r="H74" s="45"/>
+      <c r="I74" s="45"/>
+      <c r="J74" s="45"/>
+      <c r="K74" s="46"/>
       <c r="L74" s="3"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12">
       <c r="A75" s="1"/>
       <c r="B75" s="3"/>
       <c r="C75" s="17"/>
       <c r="D75" s="6"/>
-      <c r="E75" s="53"/>
-      <c r="F75" s="44"/>
-      <c r="G75" s="30"/>
-      <c r="H75" s="35"/>
-      <c r="I75" s="35"/>
-      <c r="J75" s="35"/>
-      <c r="K75" s="31"/>
+      <c r="E75" s="67"/>
+      <c r="F75" s="68"/>
+      <c r="G75" s="44"/>
+      <c r="H75" s="45"/>
+      <c r="I75" s="45"/>
+      <c r="J75" s="45"/>
+      <c r="K75" s="46"/>
       <c r="L75" s="3"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12">
       <c r="A76" s="1"/>
       <c r="B76" s="3"/>
       <c r="C76" s="18" t="s">
@@ -4334,44 +4344,44 @@
       <c r="D76" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E76" s="54"/>
-      <c r="F76" s="55"/>
-      <c r="G76" s="30"/>
-      <c r="H76" s="35"/>
-      <c r="I76" s="35"/>
-      <c r="J76" s="35"/>
-      <c r="K76" s="31"/>
+      <c r="E76" s="69"/>
+      <c r="F76" s="70"/>
+      <c r="G76" s="44"/>
+      <c r="H76" s="45"/>
+      <c r="I76" s="45"/>
+      <c r="J76" s="45"/>
+      <c r="K76" s="46"/>
       <c r="L76" s="3"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12">
       <c r="A77" s="1"/>
       <c r="B77" s="3"/>
       <c r="C77" s="15"/>
       <c r="D77" s="3"/>
-      <c r="E77" s="54"/>
-      <c r="F77" s="55"/>
-      <c r="G77" s="30"/>
-      <c r="H77" s="35"/>
-      <c r="I77" s="35"/>
-      <c r="J77" s="35"/>
-      <c r="K77" s="31"/>
+      <c r="E77" s="69"/>
+      <c r="F77" s="70"/>
+      <c r="G77" s="44"/>
+      <c r="H77" s="45"/>
+      <c r="I77" s="45"/>
+      <c r="J77" s="45"/>
+      <c r="K77" s="46"/>
       <c r="L77" s="3"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12">
       <c r="A78" s="1"/>
       <c r="B78" s="3"/>
       <c r="C78" s="17"/>
       <c r="D78" s="3"/>
-      <c r="E78" s="54"/>
-      <c r="F78" s="55"/>
-      <c r="G78" s="30"/>
-      <c r="H78" s="35"/>
-      <c r="I78" s="35"/>
-      <c r="J78" s="35"/>
-      <c r="K78" s="31"/>
+      <c r="E78" s="69"/>
+      <c r="F78" s="70"/>
+      <c r="G78" s="44"/>
+      <c r="H78" s="45"/>
+      <c r="I78" s="45"/>
+      <c r="J78" s="45"/>
+      <c r="K78" s="46"/>
       <c r="L78" s="3"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12">
       <c r="A79" s="1"/>
       <c r="B79" s="3"/>
       <c r="C79" s="15" t="s">
@@ -4380,16 +4390,16 @@
       <c r="D79" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E79" s="45"/>
-      <c r="F79" s="46"/>
-      <c r="G79" s="30"/>
-      <c r="H79" s="35"/>
-      <c r="I79" s="35"/>
-      <c r="J79" s="35"/>
-      <c r="K79" s="31"/>
+      <c r="E79" s="51"/>
+      <c r="F79" s="52"/>
+      <c r="G79" s="44"/>
+      <c r="H79" s="45"/>
+      <c r="I79" s="45"/>
+      <c r="J79" s="45"/>
+      <c r="K79" s="46"/>
       <c r="L79" s="3"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12">
       <c r="A80" s="1"/>
       <c r="B80" s="3"/>
       <c r="C80" s="19" t="s">
@@ -4398,16 +4408,16 @@
       <c r="D80" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E80" s="47"/>
-      <c r="F80" s="48"/>
-      <c r="G80" s="30"/>
-      <c r="H80" s="35"/>
-      <c r="I80" s="35"/>
-      <c r="J80" s="35"/>
-      <c r="K80" s="31"/>
+      <c r="E80" s="56"/>
+      <c r="F80" s="54"/>
+      <c r="G80" s="44"/>
+      <c r="H80" s="45"/>
+      <c r="I80" s="45"/>
+      <c r="J80" s="45"/>
+      <c r="K80" s="46"/>
       <c r="L80" s="3"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12">
       <c r="A81" s="1"/>
       <c r="B81" s="3"/>
       <c r="C81" s="15" t="s">
@@ -4416,16 +4426,16 @@
       <c r="D81" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E81" s="49"/>
-      <c r="F81" s="50"/>
-      <c r="G81" s="30"/>
-      <c r="H81" s="35"/>
-      <c r="I81" s="35"/>
-      <c r="J81" s="35"/>
-      <c r="K81" s="31"/>
+      <c r="E81" s="57"/>
+      <c r="F81" s="58"/>
+      <c r="G81" s="44"/>
+      <c r="H81" s="45"/>
+      <c r="I81" s="45"/>
+      <c r="J81" s="45"/>
+      <c r="K81" s="46"/>
       <c r="L81" s="3"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12">
       <c r="A82" s="1"/>
       <c r="B82" s="3"/>
       <c r="C82" s="21" t="s">
@@ -4434,16 +4444,16 @@
       <c r="D82" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E82" s="47"/>
-      <c r="F82" s="48"/>
-      <c r="G82" s="30"/>
-      <c r="H82" s="35"/>
-      <c r="I82" s="35"/>
-      <c r="J82" s="35"/>
-      <c r="K82" s="31"/>
+      <c r="E82" s="56"/>
+      <c r="F82" s="54"/>
+      <c r="G82" s="44"/>
+      <c r="H82" s="45"/>
+      <c r="I82" s="45"/>
+      <c r="J82" s="45"/>
+      <c r="K82" s="46"/>
       <c r="L82" s="3"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12">
       <c r="A83" s="1"/>
       <c r="B83" s="3"/>
       <c r="C83" s="15" t="s">
@@ -4452,16 +4462,16 @@
       <c r="D83" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E83" s="28"/>
-      <c r="F83" s="29"/>
-      <c r="G83" s="30"/>
-      <c r="H83" s="35"/>
-      <c r="I83" s="35"/>
-      <c r="J83" s="35"/>
-      <c r="K83" s="31"/>
+      <c r="E83" s="59"/>
+      <c r="F83" s="60"/>
+      <c r="G83" s="44"/>
+      <c r="H83" s="45"/>
+      <c r="I83" s="45"/>
+      <c r="J83" s="45"/>
+      <c r="K83" s="46"/>
       <c r="L83" s="3"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12">
       <c r="A84" s="1"/>
       <c r="B84" s="3"/>
       <c r="C84" s="16" t="s">
@@ -4470,51 +4480,62 @@
       <c r="D84" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E84" s="30"/>
-      <c r="F84" s="31"/>
-      <c r="G84" s="30"/>
-      <c r="H84" s="35"/>
-      <c r="I84" s="35"/>
-      <c r="J84" s="35"/>
-      <c r="K84" s="31"/>
+      <c r="E84" s="44"/>
+      <c r="F84" s="46"/>
+      <c r="G84" s="44"/>
+      <c r="H84" s="45"/>
+      <c r="I84" s="45"/>
+      <c r="J84" s="45"/>
+      <c r="K84" s="46"/>
       <c r="L84" s="3"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12">
       <c r="A85" s="5"/>
       <c r="B85" s="7"/>
       <c r="C85" s="17"/>
       <c r="D85" s="7"/>
-      <c r="E85" s="36"/>
-      <c r="F85" s="38"/>
-      <c r="G85" s="36"/>
-      <c r="H85" s="37"/>
-      <c r="I85" s="37"/>
-      <c r="J85" s="37"/>
-      <c r="K85" s="38"/>
+      <c r="E85" s="62"/>
+      <c r="F85" s="48"/>
+      <c r="G85" s="62"/>
+      <c r="H85" s="47"/>
+      <c r="I85" s="47"/>
+      <c r="J85" s="47"/>
+      <c r="K85" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="69">
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A6:B7"/>
-    <mergeCell ref="C6:F7"/>
-    <mergeCell ref="G6:K7"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="G8:K20"/>
-    <mergeCell ref="G21:K33"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E83:F83"/>
+    <mergeCell ref="E84:F84"/>
+    <mergeCell ref="G73:K85"/>
+    <mergeCell ref="E85:F85"/>
+    <mergeCell ref="E11:F13"/>
+    <mergeCell ref="E71:F71"/>
+    <mergeCell ref="E72:F72"/>
+    <mergeCell ref="E79:F79"/>
+    <mergeCell ref="E80:F80"/>
+    <mergeCell ref="E81:F81"/>
+    <mergeCell ref="E82:F82"/>
+    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="E60:F62"/>
+    <mergeCell ref="E63:F65"/>
+    <mergeCell ref="E73:F75"/>
+    <mergeCell ref="E76:F78"/>
+    <mergeCell ref="E68:F68"/>
+    <mergeCell ref="E69:F69"/>
+    <mergeCell ref="E70:F70"/>
+    <mergeCell ref="E8:F10"/>
+    <mergeCell ref="E21:F23"/>
+    <mergeCell ref="E34:F36"/>
+    <mergeCell ref="E37:F39"/>
+    <mergeCell ref="E24:F26"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E20:F20"/>
     <mergeCell ref="G60:K72"/>
     <mergeCell ref="E44:F44"/>
     <mergeCell ref="E45:F45"/>
@@ -4531,41 +4552,34 @@
     <mergeCell ref="E58:F58"/>
     <mergeCell ref="E66:F66"/>
     <mergeCell ref="E67:F67"/>
-    <mergeCell ref="E68:F68"/>
-    <mergeCell ref="E69:F69"/>
-    <mergeCell ref="E70:F70"/>
-    <mergeCell ref="E8:F10"/>
-    <mergeCell ref="E21:F23"/>
-    <mergeCell ref="E34:F36"/>
-    <mergeCell ref="E37:F39"/>
-    <mergeCell ref="E24:F26"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E83:F83"/>
-    <mergeCell ref="E84:F84"/>
-    <mergeCell ref="G73:K85"/>
-    <mergeCell ref="E85:F85"/>
-    <mergeCell ref="E11:F13"/>
-    <mergeCell ref="E71:F71"/>
-    <mergeCell ref="E72:F72"/>
-    <mergeCell ref="E79:F79"/>
-    <mergeCell ref="E80:F80"/>
-    <mergeCell ref="E81:F81"/>
-    <mergeCell ref="E82:F82"/>
-    <mergeCell ref="E59:F59"/>
-    <mergeCell ref="E60:F62"/>
-    <mergeCell ref="E63:F65"/>
-    <mergeCell ref="E73:F75"/>
-    <mergeCell ref="E76:F78"/>
+    <mergeCell ref="G8:K20"/>
+    <mergeCell ref="G21:K33"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A6:B7"/>
+    <mergeCell ref="C6:F7"/>
+    <mergeCell ref="G6:K7"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="I4:K4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>